<commit_message>
feat: post populate excel
</commit_message>
<xml_diff>
--- a/static/gamefication.xlsx
+++ b/static/gamefication.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">register</t>
   </si>
   <si>
     <t xml:space="preserve">Se cadastrou</t>
@@ -37,6 +43,9 @@
     <t xml:space="preserve">Pediu para ganhar produto ao invés de fazer doação na lista de desejos:</t>
   </si>
   <si>
+    <t xml:space="preserve">contribution</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gravou vídeo solicitando o presente:</t>
   </si>
   <si>
@@ -47,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">curiosities</t>
   </si>
   <si>
     <t xml:space="preserve">Resumo de você:</t>
@@ -137,8 +149,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -211,8 +224,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,31 +258,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C1002"/>
+  <dimension ref="B1:D1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="75.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>1.2</v>
       </c>
     </row>
@@ -273,31 +296,43 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -305,23 +340,32 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -329,39 +373,54 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="n">
         <v>0.025</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -369,3090 +428,3165 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="n">
         <v>0.025</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2" t="n">
         <v>0.075</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="n">
         <v>0.075</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="2" t="n">
         <v>0.135</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="2" t="n">
         <v>0.108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="2" t="n">
         <v>0.108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="2" t="n">
         <v>0.045</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="2" t="n">
         <v>0.075</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="2" t="n">
         <v>0.175</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="2"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="2"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="2"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="2"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="2"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="2"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="2"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="2"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="2"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="2"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="2"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="2"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="2"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="2"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="2"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="2"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="2"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="2"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="2"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="2"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="2"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="2"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C75" s="2"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="2"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="2"/>
+      <c r="D77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="2"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="2"/>
+      <c r="D79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="2"/>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C81" s="2"/>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="2"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="2"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="2"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="2"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="2"/>
+      <c r="D86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="2"/>
+      <c r="D87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="2"/>
+      <c r="D88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="2"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="2"/>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="2"/>
+      <c r="D91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="2"/>
+      <c r="D92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="2"/>
+      <c r="D93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="2"/>
+      <c r="D94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="2"/>
+      <c r="D95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C96" s="2"/>
+      <c r="D96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="2"/>
+      <c r="D97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="2"/>
+      <c r="D98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="2"/>
+      <c r="D99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="2"/>
+      <c r="D100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="2"/>
+      <c r="D101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="2"/>
+      <c r="D102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="2"/>
+      <c r="D103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="2"/>
+      <c r="D104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="2"/>
+      <c r="D105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C106" s="2"/>
+      <c r="D106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="2"/>
+      <c r="D107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="2"/>
+      <c r="D108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C109" s="2"/>
+      <c r="D109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="2"/>
+      <c r="D110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="2"/>
+      <c r="D111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="2"/>
+      <c r="D112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="2"/>
+      <c r="D113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="2"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="2"/>
+      <c r="D115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="2"/>
+      <c r="D116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="2"/>
+      <c r="D117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="2"/>
+      <c r="D118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="2"/>
+      <c r="D119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="2"/>
+      <c r="D120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="2"/>
+      <c r="D121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="2"/>
+      <c r="D122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C123" s="2"/>
+      <c r="D123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="2"/>
+      <c r="D124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C125" s="2"/>
+      <c r="D125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="2"/>
+      <c r="D127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="2"/>
+      <c r="D128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="2"/>
+      <c r="D129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="2"/>
+      <c r="D130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="2"/>
+      <c r="D131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="2"/>
+      <c r="D132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C133" s="2"/>
+      <c r="D133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="2"/>
+      <c r="D134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="2"/>
+      <c r="D135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C136" s="2"/>
+      <c r="D136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="2"/>
+      <c r="D137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="2"/>
+      <c r="D138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="2"/>
+      <c r="D139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C140" s="2"/>
+      <c r="D140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C141" s="2"/>
+      <c r="D141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="2"/>
+      <c r="D142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="2"/>
+      <c r="D143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C144" s="2"/>
+      <c r="D144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C145" s="2"/>
+      <c r="D145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C146" s="2"/>
+      <c r="D146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="2"/>
+      <c r="D147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="2"/>
+      <c r="D148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C149" s="2"/>
+      <c r="D149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="2"/>
+      <c r="D150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="2"/>
+      <c r="D151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="2"/>
+      <c r="D152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="2"/>
+      <c r="D153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="2"/>
+      <c r="D154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="2"/>
+      <c r="D155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="2"/>
+      <c r="D156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="2"/>
+      <c r="D157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="2"/>
+      <c r="D158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="2"/>
+      <c r="D159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="2"/>
+      <c r="D160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="2"/>
+      <c r="D161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="2"/>
+      <c r="D162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="2"/>
+      <c r="D163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="2"/>
+      <c r="D164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="2"/>
+      <c r="D165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="2"/>
+      <c r="D166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="2"/>
+      <c r="D167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="2"/>
+      <c r="D168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C169" s="2"/>
+      <c r="D169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="2"/>
+      <c r="D170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="2"/>
+      <c r="D171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="2"/>
+      <c r="D172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="2"/>
+      <c r="D173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="2"/>
+      <c r="D174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="2"/>
+      <c r="D175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="2"/>
+      <c r="D176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="2"/>
+      <c r="D177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="2"/>
+      <c r="D178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="2"/>
+      <c r="D179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C180" s="2"/>
+      <c r="D180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="2"/>
+      <c r="D181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="2"/>
+      <c r="D182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="2"/>
+      <c r="D183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="2"/>
+      <c r="D184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="2"/>
+      <c r="D185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="2"/>
+      <c r="D186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C187" s="2"/>
+      <c r="D187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="2"/>
+      <c r="D188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="2"/>
+      <c r="D189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="2"/>
+      <c r="D190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="2"/>
+      <c r="D191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="2"/>
+      <c r="D192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C193" s="2"/>
+      <c r="D193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="2"/>
+      <c r="D194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="2"/>
+      <c r="D195" s="3"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="2"/>
+      <c r="D196" s="3"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C197" s="2"/>
+      <c r="D197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="2"/>
+      <c r="D198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="2"/>
+      <c r="D199" s="3"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="2"/>
+      <c r="D200" s="3"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="2"/>
+      <c r="D201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="2"/>
+      <c r="D202" s="3"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="2"/>
+      <c r="D203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="2"/>
+      <c r="D204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="2"/>
+      <c r="D205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="2"/>
+      <c r="D206" s="3"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="2"/>
+      <c r="D207" s="3"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C208" s="2"/>
+      <c r="D208" s="3"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="2"/>
+      <c r="D209" s="3"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="2"/>
+      <c r="D210" s="3"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="2"/>
+      <c r="D211" s="3"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="2"/>
+      <c r="D212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="2"/>
+      <c r="D213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="2"/>
+      <c r="D214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="2"/>
+      <c r="D215" s="3"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="2"/>
+      <c r="D216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C217" s="2"/>
+      <c r="D217" s="3"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="2"/>
+      <c r="D218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="2"/>
+      <c r="D219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="2"/>
+      <c r="D220" s="3"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="2"/>
+      <c r="D221" s="3"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="2"/>
+      <c r="D222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="2"/>
+      <c r="D223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="2"/>
+      <c r="D224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="2"/>
+      <c r="D225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="2"/>
+      <c r="D226" s="3"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="2"/>
+      <c r="D227" s="3"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="2"/>
+      <c r="D228" s="3"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="2"/>
+      <c r="D229" s="3"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="2"/>
+      <c r="D230" s="3"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="2"/>
+      <c r="D231" s="3"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="2"/>
+      <c r="D232" s="3"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C233" s="2"/>
+      <c r="D233" s="3"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="2"/>
+      <c r="D234" s="3"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="2"/>
+      <c r="D235" s="3"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C236" s="2"/>
+      <c r="D236" s="3"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="2"/>
+      <c r="D237" s="3"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="2"/>
+      <c r="D238" s="3"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C239" s="2"/>
+      <c r="D239" s="3"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="2"/>
+      <c r="D240" s="3"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="2"/>
+      <c r="D241" s="3"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C242" s="2"/>
+      <c r="D242" s="3"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="2"/>
+      <c r="D243" s="3"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C244" s="2"/>
+      <c r="D244" s="3"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C245" s="2"/>
+      <c r="D245" s="3"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C246" s="2"/>
+      <c r="D246" s="3"/>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C247" s="2"/>
+      <c r="D247" s="3"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="2"/>
+      <c r="D248" s="3"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C249" s="2"/>
+      <c r="D249" s="3"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="2"/>
+      <c r="D250" s="3"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C251" s="2"/>
+      <c r="D251" s="3"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C252" s="2"/>
+      <c r="D252" s="3"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="2"/>
+      <c r="D253" s="3"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C254" s="2"/>
+      <c r="D254" s="3"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C255" s="2"/>
+      <c r="D255" s="3"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="2"/>
+      <c r="D256" s="3"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C257" s="2"/>
+      <c r="D257" s="3"/>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C258" s="2"/>
+      <c r="D258" s="3"/>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="2"/>
+      <c r="D259" s="3"/>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C260" s="2"/>
+      <c r="D260" s="3"/>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C261" s="2"/>
+      <c r="D261" s="3"/>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="2"/>
+      <c r="D262" s="3"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C263" s="2"/>
+      <c r="D263" s="3"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="2"/>
+      <c r="D264" s="3"/>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C265" s="2"/>
+      <c r="D265" s="3"/>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C266" s="2"/>
+      <c r="D266" s="3"/>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="2"/>
+      <c r="D267" s="3"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C268" s="2"/>
+      <c r="D268" s="3"/>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C269" s="2"/>
+      <c r="D269" s="3"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="2"/>
+      <c r="D270" s="3"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="2"/>
+      <c r="D271" s="3"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="2"/>
+      <c r="D272" s="3"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C273" s="2"/>
+      <c r="D273" s="3"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="2"/>
+      <c r="D274" s="3"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C275" s="2"/>
+      <c r="D275" s="3"/>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C276" s="2"/>
+      <c r="D276" s="3"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C277" s="2"/>
+      <c r="D277" s="3"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="2"/>
+      <c r="D278" s="3"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C279" s="2"/>
+      <c r="D279" s="3"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="2"/>
+      <c r="D280" s="3"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C281" s="2"/>
+      <c r="D281" s="3"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C282" s="2"/>
+      <c r="D282" s="3"/>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="2"/>
+      <c r="D283" s="3"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C284" s="2"/>
+      <c r="D284" s="3"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="2"/>
+      <c r="D285" s="3"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="2"/>
+      <c r="D286" s="3"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="2"/>
+      <c r="D287" s="3"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="2"/>
+      <c r="D288" s="3"/>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C289" s="2"/>
+      <c r="D289" s="3"/>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="2"/>
+      <c r="D290" s="3"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C291" s="2"/>
+      <c r="D291" s="3"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C292" s="2"/>
+      <c r="D292" s="3"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C293" s="2"/>
+      <c r="D293" s="3"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C294" s="2"/>
+      <c r="D294" s="3"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="2"/>
+      <c r="D295" s="3"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C296" s="2"/>
+      <c r="D296" s="3"/>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C297" s="2"/>
+      <c r="D297" s="3"/>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="2"/>
+      <c r="D298" s="3"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C299" s="2"/>
+      <c r="D299" s="3"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C300" s="2"/>
+      <c r="D300" s="3"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C301" s="2"/>
+      <c r="D301" s="3"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C302" s="2"/>
+      <c r="D302" s="3"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C303" s="2"/>
+      <c r="D303" s="3"/>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C304" s="2"/>
+      <c r="D304" s="3"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C305" s="2"/>
+      <c r="D305" s="3"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C306" s="2"/>
+      <c r="D306" s="3"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C307" s="2"/>
+      <c r="D307" s="3"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C308" s="2"/>
+      <c r="D308" s="3"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C309" s="2"/>
+      <c r="D309" s="3"/>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="2"/>
+      <c r="D310" s="3"/>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C311" s="2"/>
+      <c r="D311" s="3"/>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C312" s="2"/>
+      <c r="D312" s="3"/>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="2"/>
+      <c r="D313" s="3"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C314" s="2"/>
+      <c r="D314" s="3"/>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C315" s="2"/>
+      <c r="D315" s="3"/>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C316" s="2"/>
+      <c r="D316" s="3"/>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C317" s="2"/>
+      <c r="D317" s="3"/>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C318" s="2"/>
+      <c r="D318" s="3"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C319" s="2"/>
+      <c r="D319" s="3"/>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C320" s="2"/>
+      <c r="D320" s="3"/>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C321" s="2"/>
+      <c r="D321" s="3"/>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C322" s="2"/>
+      <c r="D322" s="3"/>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C323" s="2"/>
+      <c r="D323" s="3"/>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C324" s="2"/>
+      <c r="D324" s="3"/>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C325" s="2"/>
+      <c r="D325" s="3"/>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C326" s="2"/>
+      <c r="D326" s="3"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C327" s="2"/>
+      <c r="D327" s="3"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C328" s="2"/>
+      <c r="D328" s="3"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C329" s="2"/>
+      <c r="D329" s="3"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C330" s="2"/>
+      <c r="D330" s="3"/>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C331" s="2"/>
+      <c r="D331" s="3"/>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C332" s="2"/>
+      <c r="D332" s="3"/>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C333" s="2"/>
+      <c r="D333" s="3"/>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C334" s="2"/>
+      <c r="D334" s="3"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C335" s="2"/>
+      <c r="D335" s="3"/>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C336" s="2"/>
+      <c r="D336" s="3"/>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C337" s="2"/>
+      <c r="D337" s="3"/>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C338" s="2"/>
+      <c r="D338" s="3"/>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C339" s="2"/>
+      <c r="D339" s="3"/>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C340" s="2"/>
+      <c r="D340" s="3"/>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="2"/>
+      <c r="D341" s="3"/>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C342" s="2"/>
+      <c r="D342" s="3"/>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C343" s="2"/>
+      <c r="D343" s="3"/>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C344" s="2"/>
+      <c r="D344" s="3"/>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C345" s="2"/>
+      <c r="D345" s="3"/>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C346" s="2"/>
+      <c r="D346" s="3"/>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C347" s="2"/>
+      <c r="D347" s="3"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C348" s="2"/>
+      <c r="D348" s="3"/>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C349" s="2"/>
+      <c r="D349" s="3"/>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C350" s="2"/>
+      <c r="D350" s="3"/>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C351" s="2"/>
+      <c r="D351" s="3"/>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C352" s="2"/>
+      <c r="D352" s="3"/>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C353" s="2"/>
+      <c r="D353" s="3"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C354" s="2"/>
+      <c r="D354" s="3"/>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C355" s="2"/>
+      <c r="D355" s="3"/>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C356" s="2"/>
+      <c r="D356" s="3"/>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C357" s="2"/>
+      <c r="D357" s="3"/>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C358" s="2"/>
+      <c r="D358" s="3"/>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C359" s="2"/>
+      <c r="D359" s="3"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C360" s="2"/>
+      <c r="D360" s="3"/>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C361" s="2"/>
+      <c r="D361" s="3"/>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C362" s="2"/>
+      <c r="D362" s="3"/>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C363" s="2"/>
+      <c r="D363" s="3"/>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C364" s="2"/>
+      <c r="D364" s="3"/>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="2"/>
+      <c r="D365" s="3"/>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C366" s="2"/>
+      <c r="D366" s="3"/>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C367" s="2"/>
+      <c r="D367" s="3"/>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C368" s="2"/>
+      <c r="D368" s="3"/>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C369" s="2"/>
+      <c r="D369" s="3"/>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C370" s="2"/>
+      <c r="D370" s="3"/>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="2"/>
+      <c r="D371" s="3"/>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C372" s="2"/>
+      <c r="D372" s="3"/>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C373" s="2"/>
+      <c r="D373" s="3"/>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C374" s="2"/>
+      <c r="D374" s="3"/>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C375" s="2"/>
+      <c r="D375" s="3"/>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C376" s="2"/>
+      <c r="D376" s="3"/>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C377" s="2"/>
+      <c r="D377" s="3"/>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C378" s="2"/>
+      <c r="D378" s="3"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C379" s="2"/>
+      <c r="D379" s="3"/>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C380" s="2"/>
+      <c r="D380" s="3"/>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C381" s="2"/>
+      <c r="D381" s="3"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C382" s="2"/>
+      <c r="D382" s="3"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C383" s="2"/>
+      <c r="D383" s="3"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C384" s="2"/>
+      <c r="D384" s="3"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C385" s="2"/>
+      <c r="D385" s="3"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C386" s="2"/>
+      <c r="D386" s="3"/>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C387" s="2"/>
+      <c r="D387" s="3"/>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C388" s="2"/>
+      <c r="D388" s="3"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C389" s="2"/>
+      <c r="D389" s="3"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C390" s="2"/>
+      <c r="D390" s="3"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C391" s="2"/>
+      <c r="D391" s="3"/>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C392" s="2"/>
+      <c r="D392" s="3"/>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C393" s="2"/>
+      <c r="D393" s="3"/>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C394" s="2"/>
+      <c r="D394" s="3"/>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C395" s="2"/>
+      <c r="D395" s="3"/>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C396" s="2"/>
+      <c r="D396" s="3"/>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C397" s="2"/>
+      <c r="D397" s="3"/>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C398" s="2"/>
+      <c r="D398" s="3"/>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C399" s="2"/>
+      <c r="D399" s="3"/>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C400" s="2"/>
+      <c r="D400" s="3"/>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C401" s="2"/>
+      <c r="D401" s="3"/>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C402" s="2"/>
+      <c r="D402" s="3"/>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C403" s="2"/>
+      <c r="D403" s="3"/>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C404" s="2"/>
+      <c r="D404" s="3"/>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C405" s="2"/>
+      <c r="D405" s="3"/>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C406" s="2"/>
+      <c r="D406" s="3"/>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C407" s="2"/>
+      <c r="D407" s="3"/>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C408" s="2"/>
+      <c r="D408" s="3"/>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C409" s="2"/>
+      <c r="D409" s="3"/>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C410" s="2"/>
+      <c r="D410" s="3"/>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C411" s="2"/>
+      <c r="D411" s="3"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C412" s="2"/>
+      <c r="D412" s="3"/>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C413" s="2"/>
+      <c r="D413" s="3"/>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C414" s="2"/>
+      <c r="D414" s="3"/>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C415" s="2"/>
+      <c r="D415" s="3"/>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C416" s="2"/>
+      <c r="D416" s="3"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C417" s="2"/>
+      <c r="D417" s="3"/>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C418" s="2"/>
+      <c r="D418" s="3"/>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C419" s="2"/>
+      <c r="D419" s="3"/>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C420" s="2"/>
+      <c r="D420" s="3"/>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C421" s="2"/>
+      <c r="D421" s="3"/>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C422" s="2"/>
+      <c r="D422" s="3"/>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C423" s="2"/>
+      <c r="D423" s="3"/>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C424" s="2"/>
+      <c r="D424" s="3"/>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C425" s="2"/>
+      <c r="D425" s="3"/>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C426" s="2"/>
+      <c r="D426" s="3"/>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C427" s="2"/>
+      <c r="D427" s="3"/>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="2"/>
+      <c r="D428" s="3"/>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C429" s="2"/>
+      <c r="D429" s="3"/>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="2"/>
+      <c r="D430" s="3"/>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C431" s="2"/>
+      <c r="D431" s="3"/>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C432" s="2"/>
+      <c r="D432" s="3"/>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C433" s="2"/>
+      <c r="D433" s="3"/>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C434" s="2"/>
+      <c r="D434" s="3"/>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C435" s="2"/>
+      <c r="D435" s="3"/>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C436" s="2"/>
+      <c r="D436" s="3"/>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C437" s="2"/>
+      <c r="D437" s="3"/>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C438" s="2"/>
+      <c r="D438" s="3"/>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C439" s="2"/>
+      <c r="D439" s="3"/>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C440" s="2"/>
+      <c r="D440" s="3"/>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C441" s="2"/>
+      <c r="D441" s="3"/>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C442" s="2"/>
+      <c r="D442" s="3"/>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C443" s="2"/>
+      <c r="D443" s="3"/>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C444" s="2"/>
+      <c r="D444" s="3"/>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C445" s="2"/>
+      <c r="D445" s="3"/>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C446" s="2"/>
+      <c r="D446" s="3"/>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C447" s="2"/>
+      <c r="D447" s="3"/>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C448" s="2"/>
+      <c r="D448" s="3"/>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C449" s="2"/>
+      <c r="D449" s="3"/>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C450" s="2"/>
+      <c r="D450" s="3"/>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C451" s="2"/>
+      <c r="D451" s="3"/>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C452" s="2"/>
+      <c r="D452" s="3"/>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C453" s="2"/>
+      <c r="D453" s="3"/>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C454" s="2"/>
+      <c r="D454" s="3"/>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C455" s="2"/>
+      <c r="D455" s="3"/>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C456" s="2"/>
+      <c r="D456" s="3"/>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C457" s="2"/>
+      <c r="D457" s="3"/>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C458" s="2"/>
+      <c r="D458" s="3"/>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C459" s="2"/>
+      <c r="D459" s="3"/>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C460" s="2"/>
+      <c r="D460" s="3"/>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C461" s="2"/>
+      <c r="D461" s="3"/>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C462" s="2"/>
+      <c r="D462" s="3"/>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C463" s="2"/>
+      <c r="D463" s="3"/>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C464" s="2"/>
+      <c r="D464" s="3"/>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C465" s="2"/>
+      <c r="D465" s="3"/>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C466" s="2"/>
+      <c r="D466" s="3"/>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C467" s="2"/>
+      <c r="D467" s="3"/>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C468" s="2"/>
+      <c r="D468" s="3"/>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C469" s="2"/>
+      <c r="D469" s="3"/>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C470" s="2"/>
+      <c r="D470" s="3"/>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C471" s="2"/>
+      <c r="D471" s="3"/>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C472" s="2"/>
+      <c r="D472" s="3"/>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C473" s="2"/>
+      <c r="D473" s="3"/>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C474" s="2"/>
+      <c r="D474" s="3"/>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C475" s="2"/>
+      <c r="D475" s="3"/>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C476" s="2"/>
+      <c r="D476" s="3"/>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C477" s="2"/>
+      <c r="D477" s="3"/>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C478" s="2"/>
+      <c r="D478" s="3"/>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C479" s="2"/>
+      <c r="D479" s="3"/>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C480" s="2"/>
+      <c r="D480" s="3"/>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C481" s="2"/>
+      <c r="D481" s="3"/>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C482" s="2"/>
+      <c r="D482" s="3"/>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C483" s="2"/>
+      <c r="D483" s="3"/>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C484" s="2"/>
+      <c r="D484" s="3"/>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C485" s="2"/>
+      <c r="D485" s="3"/>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C486" s="2"/>
+      <c r="D486" s="3"/>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C487" s="2"/>
+      <c r="D487" s="3"/>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C488" s="2"/>
+      <c r="D488" s="3"/>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C489" s="2"/>
+      <c r="D489" s="3"/>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C490" s="2"/>
+      <c r="D490" s="3"/>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C491" s="2"/>
+      <c r="D491" s="3"/>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C492" s="2"/>
+      <c r="D492" s="3"/>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C493" s="2"/>
+      <c r="D493" s="3"/>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C494" s="2"/>
+      <c r="D494" s="3"/>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="2"/>
+      <c r="D495" s="3"/>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C496" s="2"/>
+      <c r="D496" s="3"/>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C497" s="2"/>
+      <c r="D497" s="3"/>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C498" s="2"/>
+      <c r="D498" s="3"/>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C499" s="2"/>
+      <c r="D499" s="3"/>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C500" s="2"/>
+      <c r="D500" s="3"/>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C501" s="2"/>
+      <c r="D501" s="3"/>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C502" s="2"/>
+      <c r="D502" s="3"/>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C503" s="2"/>
+      <c r="D503" s="3"/>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C504" s="2"/>
+      <c r="D504" s="3"/>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C505" s="2"/>
+      <c r="D505" s="3"/>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C506" s="2"/>
+      <c r="D506" s="3"/>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C507" s="2"/>
+      <c r="D507" s="3"/>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C508" s="2"/>
+      <c r="D508" s="3"/>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C509" s="2"/>
+      <c r="D509" s="3"/>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C510" s="2"/>
+      <c r="D510" s="3"/>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C511" s="2"/>
+      <c r="D511" s="3"/>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C512" s="2"/>
+      <c r="D512" s="3"/>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C513" s="2"/>
+      <c r="D513" s="3"/>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C514" s="2"/>
+      <c r="D514" s="3"/>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C515" s="2"/>
+      <c r="D515" s="3"/>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C516" s="2"/>
+      <c r="D516" s="3"/>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C517" s="2"/>
+      <c r="D517" s="3"/>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C518" s="2"/>
+      <c r="D518" s="3"/>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C519" s="2"/>
+      <c r="D519" s="3"/>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C520" s="2"/>
+      <c r="D520" s="3"/>
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C521" s="2"/>
+      <c r="D521" s="3"/>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C522" s="2"/>
+      <c r="D522" s="3"/>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C523" s="2"/>
+      <c r="D523" s="3"/>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C524" s="2"/>
+      <c r="D524" s="3"/>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C525" s="2"/>
+      <c r="D525" s="3"/>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C526" s="2"/>
+      <c r="D526" s="3"/>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C527" s="2"/>
+      <c r="D527" s="3"/>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C528" s="2"/>
+      <c r="D528" s="3"/>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="2"/>
+      <c r="D529" s="3"/>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C530" s="2"/>
+      <c r="D530" s="3"/>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C531" s="2"/>
+      <c r="D531" s="3"/>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C532" s="2"/>
+      <c r="D532" s="3"/>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C533" s="2"/>
+      <c r="D533" s="3"/>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C534" s="2"/>
+      <c r="D534" s="3"/>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C535" s="2"/>
+      <c r="D535" s="3"/>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C536" s="2"/>
+      <c r="D536" s="3"/>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C537" s="2"/>
+      <c r="D537" s="3"/>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C538" s="2"/>
+      <c r="D538" s="3"/>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C539" s="2"/>
+      <c r="D539" s="3"/>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C540" s="2"/>
+      <c r="D540" s="3"/>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C541" s="2"/>
+      <c r="D541" s="3"/>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C542" s="2"/>
+      <c r="D542" s="3"/>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C543" s="2"/>
+      <c r="D543" s="3"/>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C544" s="2"/>
+      <c r="D544" s="3"/>
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C545" s="2"/>
+      <c r="D545" s="3"/>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C546" s="2"/>
+      <c r="D546" s="3"/>
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C547" s="2"/>
+      <c r="D547" s="3"/>
     </row>
     <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C548" s="2"/>
+      <c r="D548" s="3"/>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C549" s="2"/>
+      <c r="D549" s="3"/>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C550" s="2"/>
+      <c r="D550" s="3"/>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C551" s="2"/>
+      <c r="D551" s="3"/>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C552" s="2"/>
+      <c r="D552" s="3"/>
     </row>
     <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C553" s="2"/>
+      <c r="D553" s="3"/>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C554" s="2"/>
+      <c r="D554" s="3"/>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C555" s="2"/>
+      <c r="D555" s="3"/>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C556" s="2"/>
+      <c r="D556" s="3"/>
     </row>
     <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C557" s="2"/>
+      <c r="D557" s="3"/>
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C558" s="2"/>
+      <c r="D558" s="3"/>
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C559" s="2"/>
+      <c r="D559" s="3"/>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C560" s="2"/>
+      <c r="D560" s="3"/>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C561" s="2"/>
+      <c r="D561" s="3"/>
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C562" s="2"/>
+      <c r="D562" s="3"/>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C563" s="2"/>
+      <c r="D563" s="3"/>
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C564" s="2"/>
+      <c r="D564" s="3"/>
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C565" s="2"/>
+      <c r="D565" s="3"/>
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C566" s="2"/>
+      <c r="D566" s="3"/>
     </row>
     <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C567" s="2"/>
+      <c r="D567" s="3"/>
     </row>
     <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C568" s="2"/>
+      <c r="D568" s="3"/>
     </row>
     <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C569" s="2"/>
+      <c r="D569" s="3"/>
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C570" s="2"/>
+      <c r="D570" s="3"/>
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C571" s="2"/>
+      <c r="D571" s="3"/>
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C572" s="2"/>
+      <c r="D572" s="3"/>
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C573" s="2"/>
+      <c r="D573" s="3"/>
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C574" s="2"/>
+      <c r="D574" s="3"/>
     </row>
     <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C575" s="2"/>
+      <c r="D575" s="3"/>
     </row>
     <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C576" s="2"/>
+      <c r="D576" s="3"/>
     </row>
     <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C577" s="2"/>
+      <c r="D577" s="3"/>
     </row>
     <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C578" s="2"/>
+      <c r="D578" s="3"/>
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C579" s="2"/>
+      <c r="D579" s="3"/>
     </row>
     <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C580" s="2"/>
+      <c r="D580" s="3"/>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C581" s="2"/>
+      <c r="D581" s="3"/>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C582" s="2"/>
+      <c r="D582" s="3"/>
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C583" s="2"/>
+      <c r="D583" s="3"/>
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C584" s="2"/>
+      <c r="D584" s="3"/>
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C585" s="2"/>
+      <c r="D585" s="3"/>
     </row>
     <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C586" s="2"/>
+      <c r="D586" s="3"/>
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C587" s="2"/>
+      <c r="D587" s="3"/>
     </row>
     <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C588" s="2"/>
+      <c r="D588" s="3"/>
     </row>
     <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C589" s="2"/>
+      <c r="D589" s="3"/>
     </row>
     <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C590" s="2"/>
+      <c r="D590" s="3"/>
     </row>
     <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C591" s="2"/>
+      <c r="D591" s="3"/>
     </row>
     <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C592" s="2"/>
+      <c r="D592" s="3"/>
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C593" s="2"/>
+      <c r="D593" s="3"/>
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C594" s="2"/>
+      <c r="D594" s="3"/>
     </row>
     <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C595" s="2"/>
+      <c r="D595" s="3"/>
     </row>
     <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C596" s="2"/>
+      <c r="D596" s="3"/>
     </row>
     <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C597" s="2"/>
+      <c r="D597" s="3"/>
     </row>
     <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C598" s="2"/>
+      <c r="D598" s="3"/>
     </row>
     <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C599" s="2"/>
+      <c r="D599" s="3"/>
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C600" s="2"/>
+      <c r="D600" s="3"/>
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C601" s="2"/>
+      <c r="D601" s="3"/>
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C602" s="2"/>
+      <c r="D602" s="3"/>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C603" s="2"/>
+      <c r="D603" s="3"/>
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C604" s="2"/>
+      <c r="D604" s="3"/>
     </row>
     <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C605" s="2"/>
+      <c r="D605" s="3"/>
     </row>
     <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C606" s="2"/>
+      <c r="D606" s="3"/>
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C607" s="2"/>
+      <c r="D607" s="3"/>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C608" s="2"/>
+      <c r="D608" s="3"/>
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C609" s="2"/>
+      <c r="D609" s="3"/>
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C610" s="2"/>
+      <c r="D610" s="3"/>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C611" s="2"/>
+      <c r="D611" s="3"/>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C612" s="2"/>
+      <c r="D612" s="3"/>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C613" s="2"/>
+      <c r="D613" s="3"/>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C614" s="2"/>
+      <c r="D614" s="3"/>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C615" s="2"/>
+      <c r="D615" s="3"/>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C616" s="2"/>
+      <c r="D616" s="3"/>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C617" s="2"/>
+      <c r="D617" s="3"/>
     </row>
     <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C618" s="2"/>
+      <c r="D618" s="3"/>
     </row>
     <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C619" s="2"/>
+      <c r="D619" s="3"/>
     </row>
     <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C620" s="2"/>
+      <c r="D620" s="3"/>
     </row>
     <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C621" s="2"/>
+      <c r="D621" s="3"/>
     </row>
     <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C622" s="2"/>
+      <c r="D622" s="3"/>
     </row>
     <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C623" s="2"/>
+      <c r="D623" s="3"/>
     </row>
     <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C624" s="2"/>
+      <c r="D624" s="3"/>
     </row>
     <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C625" s="2"/>
+      <c r="D625" s="3"/>
     </row>
     <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C626" s="2"/>
+      <c r="D626" s="3"/>
     </row>
     <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C627" s="2"/>
+      <c r="D627" s="3"/>
     </row>
     <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C628" s="2"/>
+      <c r="D628" s="3"/>
     </row>
     <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C629" s="2"/>
+      <c r="D629" s="3"/>
     </row>
     <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C630" s="2"/>
+      <c r="D630" s="3"/>
     </row>
     <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C631" s="2"/>
+      <c r="D631" s="3"/>
     </row>
     <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C632" s="2"/>
+      <c r="D632" s="3"/>
     </row>
     <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C633" s="2"/>
+      <c r="D633" s="3"/>
     </row>
     <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C634" s="2"/>
+      <c r="D634" s="3"/>
     </row>
     <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C635" s="2"/>
+      <c r="D635" s="3"/>
     </row>
     <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C636" s="2"/>
+      <c r="D636" s="3"/>
     </row>
     <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C637" s="2"/>
+      <c r="D637" s="3"/>
     </row>
     <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C638" s="2"/>
+      <c r="D638" s="3"/>
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C639" s="2"/>
+      <c r="D639" s="3"/>
     </row>
     <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C640" s="2"/>
+      <c r="D640" s="3"/>
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C641" s="2"/>
+      <c r="D641" s="3"/>
     </row>
     <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C642" s="2"/>
+      <c r="D642" s="3"/>
     </row>
     <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C643" s="2"/>
+      <c r="D643" s="3"/>
     </row>
     <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C644" s="2"/>
+      <c r="D644" s="3"/>
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C645" s="2"/>
+      <c r="D645" s="3"/>
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C646" s="2"/>
+      <c r="D646" s="3"/>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C647" s="2"/>
+      <c r="D647" s="3"/>
     </row>
     <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C648" s="2"/>
+      <c r="D648" s="3"/>
     </row>
     <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C649" s="2"/>
+      <c r="D649" s="3"/>
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C650" s="2"/>
+      <c r="D650" s="3"/>
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C651" s="2"/>
+      <c r="D651" s="3"/>
     </row>
     <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C652" s="2"/>
+      <c r="D652" s="3"/>
     </row>
     <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C653" s="2"/>
+      <c r="D653" s="3"/>
     </row>
     <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C654" s="2"/>
+      <c r="D654" s="3"/>
     </row>
     <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C655" s="2"/>
+      <c r="D655" s="3"/>
     </row>
     <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C656" s="2"/>
+      <c r="D656" s="3"/>
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C657" s="2"/>
+      <c r="D657" s="3"/>
     </row>
     <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C658" s="2"/>
+      <c r="D658" s="3"/>
     </row>
     <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C659" s="2"/>
+      <c r="D659" s="3"/>
     </row>
     <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C660" s="2"/>
+      <c r="D660" s="3"/>
     </row>
     <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C661" s="2"/>
+      <c r="D661" s="3"/>
     </row>
     <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C662" s="2"/>
+      <c r="D662" s="3"/>
     </row>
     <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C663" s="2"/>
+      <c r="D663" s="3"/>
     </row>
     <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C664" s="2"/>
+      <c r="D664" s="3"/>
     </row>
     <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C665" s="2"/>
+      <c r="D665" s="3"/>
     </row>
     <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C666" s="2"/>
+      <c r="D666" s="3"/>
     </row>
     <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C667" s="2"/>
+      <c r="D667" s="3"/>
     </row>
     <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C668" s="2"/>
+      <c r="D668" s="3"/>
     </row>
     <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C669" s="2"/>
+      <c r="D669" s="3"/>
     </row>
     <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C670" s="2"/>
+      <c r="D670" s="3"/>
     </row>
     <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C671" s="2"/>
+      <c r="D671" s="3"/>
     </row>
     <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C672" s="2"/>
+      <c r="D672" s="3"/>
     </row>
     <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C673" s="2"/>
+      <c r="D673" s="3"/>
     </row>
     <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C674" s="2"/>
+      <c r="D674" s="3"/>
     </row>
     <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C675" s="2"/>
+      <c r="D675" s="3"/>
     </row>
     <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C676" s="2"/>
+      <c r="D676" s="3"/>
     </row>
     <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C677" s="2"/>
+      <c r="D677" s="3"/>
     </row>
     <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C678" s="2"/>
+      <c r="D678" s="3"/>
     </row>
     <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C679" s="2"/>
+      <c r="D679" s="3"/>
     </row>
     <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C680" s="2"/>
+      <c r="D680" s="3"/>
     </row>
     <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C681" s="2"/>
+      <c r="D681" s="3"/>
     </row>
     <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C682" s="2"/>
+      <c r="D682" s="3"/>
     </row>
     <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C683" s="2"/>
+      <c r="D683" s="3"/>
     </row>
     <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C684" s="2"/>
+      <c r="D684" s="3"/>
     </row>
     <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C685" s="2"/>
+      <c r="D685" s="3"/>
     </row>
     <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C686" s="2"/>
+      <c r="D686" s="3"/>
     </row>
     <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C687" s="2"/>
+      <c r="D687" s="3"/>
     </row>
     <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C688" s="2"/>
+      <c r="D688" s="3"/>
     </row>
     <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C689" s="2"/>
+      <c r="D689" s="3"/>
     </row>
     <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C690" s="2"/>
+      <c r="D690" s="3"/>
     </row>
     <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C691" s="2"/>
+      <c r="D691" s="3"/>
     </row>
     <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C692" s="2"/>
+      <c r="D692" s="3"/>
     </row>
     <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C693" s="2"/>
+      <c r="D693" s="3"/>
     </row>
     <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C694" s="2"/>
+      <c r="D694" s="3"/>
     </row>
     <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C695" s="2"/>
+      <c r="D695" s="3"/>
     </row>
     <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C696" s="2"/>
+      <c r="D696" s="3"/>
     </row>
     <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C697" s="2"/>
+      <c r="D697" s="3"/>
     </row>
     <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C698" s="2"/>
+      <c r="D698" s="3"/>
     </row>
     <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C699" s="2"/>
+      <c r="D699" s="3"/>
     </row>
     <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C700" s="2"/>
+      <c r="D700" s="3"/>
     </row>
     <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C701" s="2"/>
+      <c r="D701" s="3"/>
     </row>
     <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C702" s="2"/>
+      <c r="D702" s="3"/>
     </row>
     <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C703" s="2"/>
+      <c r="D703" s="3"/>
     </row>
     <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C704" s="2"/>
+      <c r="D704" s="3"/>
     </row>
     <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C705" s="2"/>
+      <c r="D705" s="3"/>
     </row>
     <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C706" s="2"/>
+      <c r="D706" s="3"/>
     </row>
     <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C707" s="2"/>
+      <c r="D707" s="3"/>
     </row>
     <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C708" s="2"/>
+      <c r="D708" s="3"/>
     </row>
     <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C709" s="2"/>
+      <c r="D709" s="3"/>
     </row>
     <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C710" s="2"/>
+      <c r="D710" s="3"/>
     </row>
     <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C711" s="2"/>
+      <c r="D711" s="3"/>
     </row>
     <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C712" s="2"/>
+      <c r="D712" s="3"/>
     </row>
     <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C713" s="2"/>
+      <c r="D713" s="3"/>
     </row>
     <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C714" s="2"/>
+      <c r="D714" s="3"/>
     </row>
     <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C715" s="2"/>
+      <c r="D715" s="3"/>
     </row>
     <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C716" s="2"/>
+      <c r="D716" s="3"/>
     </row>
     <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C717" s="2"/>
+      <c r="D717" s="3"/>
     </row>
     <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C718" s="2"/>
+      <c r="D718" s="3"/>
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C719" s="2"/>
+      <c r="D719" s="3"/>
     </row>
     <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C720" s="2"/>
+      <c r="D720" s="3"/>
     </row>
     <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C721" s="2"/>
+      <c r="D721" s="3"/>
     </row>
     <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C722" s="2"/>
+      <c r="D722" s="3"/>
     </row>
     <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C723" s="2"/>
+      <c r="D723" s="3"/>
     </row>
     <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C724" s="2"/>
+      <c r="D724" s="3"/>
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C725" s="2"/>
+      <c r="D725" s="3"/>
     </row>
     <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C726" s="2"/>
+      <c r="D726" s="3"/>
     </row>
     <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C727" s="2"/>
+      <c r="D727" s="3"/>
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C728" s="2"/>
+      <c r="D728" s="3"/>
     </row>
     <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C729" s="2"/>
+      <c r="D729" s="3"/>
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C730" s="2"/>
+      <c r="D730" s="3"/>
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C731" s="2"/>
+      <c r="D731" s="3"/>
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C732" s="2"/>
+      <c r="D732" s="3"/>
     </row>
     <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C733" s="2"/>
+      <c r="D733" s="3"/>
     </row>
     <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C734" s="2"/>
+      <c r="D734" s="3"/>
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C735" s="2"/>
+      <c r="D735" s="3"/>
     </row>
     <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C736" s="2"/>
+      <c r="D736" s="3"/>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C737" s="2"/>
+      <c r="D737" s="3"/>
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C738" s="2"/>
+      <c r="D738" s="3"/>
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C739" s="2"/>
+      <c r="D739" s="3"/>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C740" s="2"/>
+      <c r="D740" s="3"/>
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C741" s="2"/>
+      <c r="D741" s="3"/>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C742" s="2"/>
+      <c r="D742" s="3"/>
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C743" s="2"/>
+      <c r="D743" s="3"/>
     </row>
     <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C744" s="2"/>
+      <c r="D744" s="3"/>
     </row>
     <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C745" s="2"/>
+      <c r="D745" s="3"/>
     </row>
     <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C746" s="2"/>
+      <c r="D746" s="3"/>
     </row>
     <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C747" s="2"/>
+      <c r="D747" s="3"/>
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C748" s="2"/>
+      <c r="D748" s="3"/>
     </row>
     <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C749" s="2"/>
+      <c r="D749" s="3"/>
     </row>
     <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C750" s="2"/>
+      <c r="D750" s="3"/>
     </row>
     <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C751" s="2"/>
+      <c r="D751" s="3"/>
     </row>
     <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C752" s="2"/>
+      <c r="D752" s="3"/>
     </row>
     <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C753" s="2"/>
+      <c r="D753" s="3"/>
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C754" s="2"/>
+      <c r="D754" s="3"/>
     </row>
     <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C755" s="2"/>
+      <c r="D755" s="3"/>
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C756" s="2"/>
+      <c r="D756" s="3"/>
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C757" s="2"/>
+      <c r="D757" s="3"/>
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C758" s="2"/>
+      <c r="D758" s="3"/>
     </row>
     <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C759" s="2"/>
+      <c r="D759" s="3"/>
     </row>
     <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C760" s="2"/>
+      <c r="D760" s="3"/>
     </row>
     <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C761" s="2"/>
+      <c r="D761" s="3"/>
     </row>
     <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C762" s="2"/>
+      <c r="D762" s="3"/>
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C763" s="2"/>
+      <c r="D763" s="3"/>
     </row>
     <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C764" s="2"/>
+      <c r="D764" s="3"/>
     </row>
     <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C765" s="2"/>
+      <c r="D765" s="3"/>
     </row>
     <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C766" s="2"/>
+      <c r="D766" s="3"/>
     </row>
     <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C767" s="2"/>
+      <c r="D767" s="3"/>
     </row>
     <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C768" s="2"/>
+      <c r="D768" s="3"/>
     </row>
     <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C769" s="2"/>
+      <c r="D769" s="3"/>
     </row>
     <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C770" s="2"/>
+      <c r="D770" s="3"/>
     </row>
     <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C771" s="2"/>
+      <c r="D771" s="3"/>
     </row>
     <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C772" s="2"/>
+      <c r="D772" s="3"/>
     </row>
     <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C773" s="2"/>
+      <c r="D773" s="3"/>
     </row>
     <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C774" s="2"/>
+      <c r="D774" s="3"/>
     </row>
     <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C775" s="2"/>
+      <c r="D775" s="3"/>
     </row>
     <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C776" s="2"/>
+      <c r="D776" s="3"/>
     </row>
     <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C777" s="2"/>
+      <c r="D777" s="3"/>
     </row>
     <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C778" s="2"/>
+      <c r="D778" s="3"/>
     </row>
     <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C779" s="2"/>
+      <c r="D779" s="3"/>
     </row>
     <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C780" s="2"/>
+      <c r="D780" s="3"/>
     </row>
     <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C781" s="2"/>
+      <c r="D781" s="3"/>
     </row>
     <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C782" s="2"/>
+      <c r="D782" s="3"/>
     </row>
     <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C783" s="2"/>
+      <c r="D783" s="3"/>
     </row>
     <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C784" s="2"/>
+      <c r="D784" s="3"/>
     </row>
     <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C785" s="2"/>
+      <c r="D785" s="3"/>
     </row>
     <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C786" s="2"/>
+      <c r="D786" s="3"/>
     </row>
     <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C787" s="2"/>
+      <c r="D787" s="3"/>
     </row>
     <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C788" s="2"/>
+      <c r="D788" s="3"/>
     </row>
     <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C789" s="2"/>
+      <c r="D789" s="3"/>
     </row>
     <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C790" s="2"/>
+      <c r="D790" s="3"/>
     </row>
     <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C791" s="2"/>
+      <c r="D791" s="3"/>
     </row>
     <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C792" s="2"/>
+      <c r="D792" s="3"/>
     </row>
     <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C793" s="2"/>
+      <c r="D793" s="3"/>
     </row>
     <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C794" s="2"/>
+      <c r="D794" s="3"/>
     </row>
     <row r="795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C795" s="2"/>
+      <c r="D795" s="3"/>
     </row>
     <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C796" s="2"/>
+      <c r="D796" s="3"/>
     </row>
     <row r="797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C797" s="2"/>
+      <c r="D797" s="3"/>
     </row>
     <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C798" s="2"/>
+      <c r="D798" s="3"/>
     </row>
     <row r="799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C799" s="2"/>
+      <c r="D799" s="3"/>
     </row>
     <row r="800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C800" s="2"/>
+      <c r="D800" s="3"/>
     </row>
     <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C801" s="2"/>
+      <c r="D801" s="3"/>
     </row>
     <row r="802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C802" s="2"/>
+      <c r="D802" s="3"/>
     </row>
     <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C803" s="2"/>
+      <c r="D803" s="3"/>
     </row>
     <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C804" s="2"/>
+      <c r="D804" s="3"/>
     </row>
     <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C805" s="2"/>
+      <c r="D805" s="3"/>
     </row>
     <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C806" s="2"/>
+      <c r="D806" s="3"/>
     </row>
     <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C807" s="2"/>
+      <c r="D807" s="3"/>
     </row>
     <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C808" s="2"/>
+      <c r="D808" s="3"/>
     </row>
     <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C809" s="2"/>
+      <c r="D809" s="3"/>
     </row>
     <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C810" s="2"/>
+      <c r="D810" s="3"/>
     </row>
     <row r="811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C811" s="2"/>
+      <c r="D811" s="3"/>
     </row>
     <row r="812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C812" s="2"/>
+      <c r="D812" s="3"/>
     </row>
     <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C813" s="2"/>
+      <c r="D813" s="3"/>
     </row>
     <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C814" s="2"/>
+      <c r="D814" s="3"/>
     </row>
     <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C815" s="2"/>
+      <c r="D815" s="3"/>
     </row>
     <row r="816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C816" s="2"/>
+      <c r="D816" s="3"/>
     </row>
     <row r="817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C817" s="2"/>
+      <c r="D817" s="3"/>
     </row>
     <row r="818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C818" s="2"/>
+      <c r="D818" s="3"/>
     </row>
     <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C819" s="2"/>
+      <c r="D819" s="3"/>
     </row>
     <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C820" s="2"/>
+      <c r="D820" s="3"/>
     </row>
     <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C821" s="2"/>
+      <c r="D821" s="3"/>
     </row>
     <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C822" s="2"/>
+      <c r="D822" s="3"/>
     </row>
     <row r="823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C823" s="2"/>
+      <c r="D823" s="3"/>
     </row>
     <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C824" s="2"/>
+      <c r="D824" s="3"/>
     </row>
     <row r="825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C825" s="2"/>
+      <c r="D825" s="3"/>
     </row>
     <row r="826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C826" s="2"/>
+      <c r="D826" s="3"/>
     </row>
     <row r="827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C827" s="2"/>
+      <c r="D827" s="3"/>
     </row>
     <row r="828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C828" s="2"/>
+      <c r="D828" s="3"/>
     </row>
     <row r="829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C829" s="2"/>
+      <c r="D829" s="3"/>
     </row>
     <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C830" s="2"/>
+      <c r="D830" s="3"/>
     </row>
     <row r="831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C831" s="2"/>
+      <c r="D831" s="3"/>
     </row>
     <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C832" s="2"/>
+      <c r="D832" s="3"/>
     </row>
     <row r="833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C833" s="2"/>
+      <c r="D833" s="3"/>
     </row>
     <row r="834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C834" s="2"/>
+      <c r="D834" s="3"/>
     </row>
     <row r="835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C835" s="2"/>
+      <c r="D835" s="3"/>
     </row>
     <row r="836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C836" s="2"/>
+      <c r="D836" s="3"/>
     </row>
     <row r="837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C837" s="2"/>
+      <c r="D837" s="3"/>
     </row>
     <row r="838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C838" s="2"/>
+      <c r="D838" s="3"/>
     </row>
     <row r="839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C839" s="2"/>
+      <c r="D839" s="3"/>
     </row>
     <row r="840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C840" s="2"/>
+      <c r="D840" s="3"/>
     </row>
     <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C841" s="2"/>
+      <c r="D841" s="3"/>
     </row>
     <row r="842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C842" s="2"/>
+      <c r="D842" s="3"/>
     </row>
     <row r="843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C843" s="2"/>
+      <c r="D843" s="3"/>
     </row>
     <row r="844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C844" s="2"/>
+      <c r="D844" s="3"/>
     </row>
     <row r="845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C845" s="2"/>
+      <c r="D845" s="3"/>
     </row>
     <row r="846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C846" s="2"/>
+      <c r="D846" s="3"/>
     </row>
     <row r="847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C847" s="2"/>
+      <c r="D847" s="3"/>
     </row>
     <row r="848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C848" s="2"/>
+      <c r="D848" s="3"/>
     </row>
     <row r="849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C849" s="2"/>
+      <c r="D849" s="3"/>
     </row>
     <row r="850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C850" s="2"/>
+      <c r="D850" s="3"/>
     </row>
     <row r="851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C851" s="2"/>
+      <c r="D851" s="3"/>
     </row>
     <row r="852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C852" s="2"/>
+      <c r="D852" s="3"/>
     </row>
     <row r="853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C853" s="2"/>
+      <c r="D853" s="3"/>
     </row>
     <row r="854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C854" s="2"/>
+      <c r="D854" s="3"/>
     </row>
     <row r="855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C855" s="2"/>
+      <c r="D855" s="3"/>
     </row>
     <row r="856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C856" s="2"/>
+      <c r="D856" s="3"/>
     </row>
     <row r="857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C857" s="2"/>
+      <c r="D857" s="3"/>
     </row>
     <row r="858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C858" s="2"/>
+      <c r="D858" s="3"/>
     </row>
     <row r="859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C859" s="2"/>
+      <c r="D859" s="3"/>
     </row>
     <row r="860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C860" s="2"/>
+      <c r="D860" s="3"/>
     </row>
     <row r="861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C861" s="2"/>
+      <c r="D861" s="3"/>
     </row>
     <row r="862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C862" s="2"/>
+      <c r="D862" s="3"/>
     </row>
     <row r="863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C863" s="2"/>
+      <c r="D863" s="3"/>
     </row>
     <row r="864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C864" s="2"/>
+      <c r="D864" s="3"/>
     </row>
     <row r="865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C865" s="2"/>
+      <c r="D865" s="3"/>
     </row>
     <row r="866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C866" s="2"/>
+      <c r="D866" s="3"/>
     </row>
     <row r="867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C867" s="2"/>
+      <c r="D867" s="3"/>
     </row>
     <row r="868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C868" s="2"/>
+      <c r="D868" s="3"/>
     </row>
     <row r="869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C869" s="2"/>
+      <c r="D869" s="3"/>
     </row>
     <row r="870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C870" s="2"/>
+      <c r="D870" s="3"/>
     </row>
     <row r="871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C871" s="2"/>
+      <c r="D871" s="3"/>
     </row>
     <row r="872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C872" s="2"/>
+      <c r="D872" s="3"/>
     </row>
     <row r="873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C873" s="2"/>
+      <c r="D873" s="3"/>
     </row>
     <row r="874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C874" s="2"/>
+      <c r="D874" s="3"/>
     </row>
     <row r="875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C875" s="2"/>
+      <c r="D875" s="3"/>
     </row>
     <row r="876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C876" s="2"/>
+      <c r="D876" s="3"/>
     </row>
     <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C877" s="2"/>
+      <c r="D877" s="3"/>
     </row>
     <row r="878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C878" s="2"/>
+      <c r="D878" s="3"/>
     </row>
     <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C879" s="2"/>
+      <c r="D879" s="3"/>
     </row>
     <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C880" s="2"/>
+      <c r="D880" s="3"/>
     </row>
     <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C881" s="2"/>
+      <c r="D881" s="3"/>
     </row>
     <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C882" s="2"/>
+      <c r="D882" s="3"/>
     </row>
     <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C883" s="2"/>
+      <c r="D883" s="3"/>
     </row>
     <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C884" s="2"/>
+      <c r="D884" s="3"/>
     </row>
     <row r="885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C885" s="2"/>
+      <c r="D885" s="3"/>
     </row>
     <row r="886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C886" s="2"/>
+      <c r="D886" s="3"/>
     </row>
     <row r="887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C887" s="2"/>
+      <c r="D887" s="3"/>
     </row>
     <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C888" s="2"/>
+      <c r="D888" s="3"/>
     </row>
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C889" s="2"/>
+      <c r="D889" s="3"/>
     </row>
     <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C890" s="2"/>
+      <c r="D890" s="3"/>
     </row>
     <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C891" s="2"/>
+      <c r="D891" s="3"/>
     </row>
     <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C892" s="2"/>
+      <c r="D892" s="3"/>
     </row>
     <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C893" s="2"/>
+      <c r="D893" s="3"/>
     </row>
     <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C894" s="2"/>
+      <c r="D894" s="3"/>
     </row>
     <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C895" s="2"/>
+      <c r="D895" s="3"/>
     </row>
     <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C896" s="2"/>
+      <c r="D896" s="3"/>
     </row>
     <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C897" s="2"/>
+      <c r="D897" s="3"/>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C898" s="2"/>
+      <c r="D898" s="3"/>
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C899" s="2"/>
+      <c r="D899" s="3"/>
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C900" s="2"/>
+      <c r="D900" s="3"/>
     </row>
     <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C901" s="2"/>
+      <c r="D901" s="3"/>
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C902" s="2"/>
+      <c r="D902" s="3"/>
     </row>
     <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C903" s="2"/>
+      <c r="D903" s="3"/>
     </row>
     <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C904" s="2"/>
+      <c r="D904" s="3"/>
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C905" s="2"/>
+      <c r="D905" s="3"/>
     </row>
     <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C906" s="2"/>
+      <c r="D906" s="3"/>
     </row>
     <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C907" s="2"/>
+      <c r="D907" s="3"/>
     </row>
     <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C908" s="2"/>
+      <c r="D908" s="3"/>
     </row>
     <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C909" s="2"/>
+      <c r="D909" s="3"/>
     </row>
     <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C910" s="2"/>
+      <c r="D910" s="3"/>
     </row>
     <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C911" s="2"/>
+      <c r="D911" s="3"/>
     </row>
     <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C912" s="2"/>
+      <c r="D912" s="3"/>
     </row>
     <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C913" s="2"/>
+      <c r="D913" s="3"/>
     </row>
     <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C914" s="2"/>
+      <c r="D914" s="3"/>
     </row>
     <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C915" s="2"/>
+      <c r="D915" s="3"/>
     </row>
     <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C916" s="2"/>
+      <c r="D916" s="3"/>
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C917" s="2"/>
+      <c r="D917" s="3"/>
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C918" s="2"/>
+      <c r="D918" s="3"/>
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C919" s="2"/>
+      <c r="D919" s="3"/>
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C920" s="2"/>
+      <c r="D920" s="3"/>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C921" s="2"/>
+      <c r="D921" s="3"/>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C922" s="2"/>
+      <c r="D922" s="3"/>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C923" s="2"/>
+      <c r="D923" s="3"/>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C924" s="2"/>
+      <c r="D924" s="3"/>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C925" s="2"/>
+      <c r="D925" s="3"/>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C926" s="2"/>
+      <c r="D926" s="3"/>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C927" s="2"/>
+      <c r="D927" s="3"/>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C928" s="2"/>
+      <c r="D928" s="3"/>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C929" s="2"/>
+      <c r="D929" s="3"/>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C930" s="2"/>
+      <c r="D930" s="3"/>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C931" s="2"/>
+      <c r="D931" s="3"/>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C932" s="2"/>
+      <c r="D932" s="3"/>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C933" s="2"/>
+      <c r="D933" s="3"/>
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C934" s="2"/>
+      <c r="D934" s="3"/>
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C935" s="2"/>
+      <c r="D935" s="3"/>
     </row>
     <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C936" s="2"/>
+      <c r="D936" s="3"/>
     </row>
     <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C937" s="2"/>
+      <c r="D937" s="3"/>
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C938" s="2"/>
+      <c r="D938" s="3"/>
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C939" s="2"/>
+      <c r="D939" s="3"/>
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C940" s="2"/>
+      <c r="D940" s="3"/>
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C941" s="2"/>
+      <c r="D941" s="3"/>
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C942" s="2"/>
+      <c r="D942" s="3"/>
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C943" s="2"/>
+      <c r="D943" s="3"/>
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C944" s="2"/>
+      <c r="D944" s="3"/>
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C945" s="2"/>
+      <c r="D945" s="3"/>
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C946" s="2"/>
+      <c r="D946" s="3"/>
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C947" s="2"/>
+      <c r="D947" s="3"/>
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C948" s="2"/>
+      <c r="D948" s="3"/>
     </row>
     <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C949" s="2"/>
+      <c r="D949" s="3"/>
     </row>
     <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C950" s="2"/>
+      <c r="D950" s="3"/>
     </row>
     <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C951" s="2"/>
+      <c r="D951" s="3"/>
     </row>
     <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C952" s="2"/>
+      <c r="D952" s="3"/>
     </row>
     <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C953" s="2"/>
+      <c r="D953" s="3"/>
     </row>
     <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C954" s="2"/>
+      <c r="D954" s="3"/>
     </row>
     <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C955" s="2"/>
+      <c r="D955" s="3"/>
     </row>
     <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C956" s="2"/>
+      <c r="D956" s="3"/>
     </row>
     <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C957" s="2"/>
+      <c r="D957" s="3"/>
     </row>
     <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C958" s="2"/>
+      <c r="D958" s="3"/>
     </row>
     <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C959" s="2"/>
+      <c r="D959" s="3"/>
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C960" s="2"/>
+      <c r="D960" s="3"/>
     </row>
     <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C961" s="2"/>
+      <c r="D961" s="3"/>
     </row>
     <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C962" s="2"/>
+      <c r="D962" s="3"/>
     </row>
     <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C963" s="2"/>
+      <c r="D963" s="3"/>
     </row>
     <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C964" s="2"/>
+      <c r="D964" s="3"/>
     </row>
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C965" s="2"/>
+      <c r="D965" s="3"/>
     </row>
     <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C966" s="2"/>
+      <c r="D966" s="3"/>
     </row>
     <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C967" s="2"/>
+      <c r="D967" s="3"/>
     </row>
     <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C968" s="2"/>
+      <c r="D968" s="3"/>
     </row>
     <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C969" s="2"/>
+      <c r="D969" s="3"/>
     </row>
     <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C970" s="2"/>
+      <c r="D970" s="3"/>
     </row>
     <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C971" s="2"/>
+      <c r="D971" s="3"/>
     </row>
     <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C972" s="2"/>
+      <c r="D972" s="3"/>
     </row>
     <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C973" s="2"/>
+      <c r="D973" s="3"/>
     </row>
     <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C974" s="2"/>
+      <c r="D974" s="3"/>
     </row>
     <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C975" s="2"/>
+      <c r="D975" s="3"/>
     </row>
     <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C976" s="2"/>
+      <c r="D976" s="3"/>
     </row>
     <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C977" s="2"/>
+      <c r="D977" s="3"/>
     </row>
     <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C978" s="2"/>
+      <c r="D978" s="3"/>
     </row>
     <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C979" s="2"/>
+      <c r="D979" s="3"/>
     </row>
     <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C980" s="2"/>
+      <c r="D980" s="3"/>
     </row>
     <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C981" s="2"/>
+      <c r="D981" s="3"/>
     </row>
     <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C982" s="2"/>
+      <c r="D982" s="3"/>
     </row>
     <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C983" s="2"/>
+      <c r="D983" s="3"/>
     </row>
     <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C984" s="2"/>
+      <c r="D984" s="3"/>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C985" s="2"/>
+      <c r="D985" s="3"/>
     </row>
     <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C986" s="2"/>
+      <c r="D986" s="3"/>
     </row>
     <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C987" s="2"/>
+      <c r="D987" s="3"/>
     </row>
     <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C988" s="2"/>
+      <c r="D988" s="3"/>
     </row>
     <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C989" s="2"/>
+      <c r="D989" s="3"/>
     </row>
     <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C990" s="2"/>
+      <c r="D990" s="3"/>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C991" s="2"/>
+      <c r="D991" s="3"/>
     </row>
     <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C992" s="2"/>
+      <c r="D992" s="3"/>
     </row>
     <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C993" s="2"/>
+      <c r="D993" s="3"/>
     </row>
     <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C994" s="2"/>
+      <c r="D994" s="3"/>
     </row>
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C995" s="2"/>
+      <c r="D995" s="3"/>
     </row>
     <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C996" s="2"/>
+      <c r="D996" s="3"/>
     </row>
     <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C997" s="2"/>
+      <c r="D997" s="3"/>
     </row>
     <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C998" s="2"/>
+      <c r="D998" s="3"/>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C999" s="2"/>
+      <c r="D999" s="3"/>
     </row>
     <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1000" s="2"/>
+      <c r="D1000" s="3"/>
     </row>
     <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1001" s="2"/>
+      <c r="D1001" s="3"/>
     </row>
     <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1002" s="2"/>
+      <c r="D1002" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>